<commit_message>
added explanation of the symbols for hypothesis statement
</commit_message>
<xml_diff>
--- a/FinalProject P1/DataSet.xlsx
+++ b/FinalProject P1/DataSet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Administrator/Documents/DataAnalyst/Statistics/FinalProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Administrator/Documents/DataAnalyst/Statistics/FinalProject P1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -878,11 +878,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="928541056"/>
-        <c:axId val="928544000"/>
+        <c:axId val="1067477024"/>
+        <c:axId val="1067481296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="928541056"/>
+        <c:axId val="1067477024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25.0"/>
@@ -976,12 +976,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="928544000"/>
+        <c:crossAx val="1067481296"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="928544000"/>
+        <c:axId val="1067481296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1088,7 +1088,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="928541056"/>
+        <c:crossAx val="1067477024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1548,11 +1548,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="895510640"/>
-        <c:axId val="895501952"/>
+        <c:axId val="1067520784"/>
+        <c:axId val="1067516752"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="895501952"/>
+        <c:axId val="1067516752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,12 +1659,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="895510640"/>
+        <c:crossAx val="1067520784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="895510640"/>
+        <c:axId val="1067520784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,7 +1757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="895501952"/>
+        <c:crossAx val="1067516752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3268,7 +3268,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>